<commit_message>
fix scorecard export & score_hist
</commit_message>
<xml_diff>
--- a/outputs/评分卡结果验证表.xlsx
+++ b/outputs/评分卡结果验证表.xlsx
@@ -8,7 +8,9 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="逻辑回归拟合结果" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="评分卡排序性" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="入模变量相关性" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="评分卡" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="评分卡排序性" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -435,11 +437,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="53" customWidth="1" min="1" max="1"/>
-    <col width="21" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="21" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
-    <col width="23" customWidth="1" min="6" max="6"/>
+    <col width="21" customWidth="1" min="6" max="6"/>
     <col width="22" customWidth="1" min="7" max="7"/>
     <col width="20" customWidth="1" min="8" max="8"/>
   </cols>
@@ -500,81 +502,81 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.844896283691845</v>
+        <v>-0.8448277696951468</v>
       </c>
       <c r="C3" t="n">
-        <v>0.09407845569373914</v>
+        <v>0.09379718050882634</v>
       </c>
       <c r="D3" t="n">
-        <v>-8.980762677932354</v>
+        <v>-9.006963376853831</v>
       </c>
       <c r="E3" t="n">
-        <v>2.688962745738168e-19</v>
+        <v>2.118407844698113e-19</v>
       </c>
       <c r="F3" t="n">
-        <v>-1.029290056851574</v>
+        <v>-1.028670243492446</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.6605025105321163</v>
+        <v>-0.6609852958978473</v>
       </c>
       <c r="H3" t="n">
-        <v>1.044894655965815</v>
+        <v>1.042857213418616</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>status.of.existing.checking.account</t>
+          <t>credit.amount</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.7775045006064929</v>
+        <v>1.026811230421579</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1288899194598336</v>
+        <v>0.2669319873384288</v>
       </c>
       <c r="D4" t="n">
-        <v>6.03231427147248</v>
+        <v>3.846714815484963</v>
       </c>
       <c r="E4" t="n">
-        <v>1.616280574457417e-09</v>
+        <v>0.0001197121739724331</v>
       </c>
       <c r="F4" t="n">
-        <v>0.524880258465219</v>
+        <v>0.5036245352382581</v>
       </c>
       <c r="G4" t="n">
-        <v>1.030128742747767</v>
+        <v>1.549997925604899</v>
       </c>
       <c r="H4" t="n">
-        <v>1.12351869752686</v>
+        <v>1.081403966880179</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>duration.in.month</t>
+          <t>installment.rate.in.percentage.of.disposable.income</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9734839926789309</v>
+        <v>1.593535550600422</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2250252309323528</v>
+        <v>0.512664846591631</v>
       </c>
       <c r="D5" t="n">
-        <v>4.326110403911017</v>
+        <v>3.10833785697378</v>
       </c>
       <c r="E5" t="n">
-        <v>1.517653773353684e-05</v>
+        <v>0.001881428515860468</v>
       </c>
       <c r="F5" t="n">
-        <v>0.5324345400515194</v>
+        <v>0.5887124512808251</v>
       </c>
       <c r="G5" t="n">
-        <v>1.414533445306343</v>
+        <v>2.598358649920018</v>
       </c>
       <c r="H5" t="n">
-        <v>1.02340712026453</v>
+        <v>1.070080627977262</v>
       </c>
     </row>
     <row r="6">
@@ -584,169 +586,167 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.6762143222032351</v>
+        <v>0.6278134710249086</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2965018058599142</v>
+        <v>0.3099752124323856</v>
       </c>
       <c r="D6" t="n">
-        <v>2.280641496405322</v>
+        <v>2.025366693350851</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0225696696707074</v>
+        <v>0.04282972484940949</v>
       </c>
       <c r="F6" t="n">
-        <v>0.09507078271780323</v>
+        <v>0.0202620546574328</v>
       </c>
       <c r="G6" t="n">
-        <v>1.257357861688667</v>
+        <v>1.235364887392384</v>
       </c>
       <c r="H6" t="n">
-        <v>1.027119563361947</v>
+        <v>1.032075451809412</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>savings.account.and.bonds</t>
+          <t>credit.history</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.718857027510439</v>
+        <v>0.6934207365944366</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2736055852691341</v>
+        <v>0.2552933638122259</v>
       </c>
       <c r="D7" t="n">
-        <v>2.627347781673865</v>
+        <v>2.716172195938722</v>
       </c>
       <c r="E7" t="n">
-        <v>0.008605333311105337</v>
+        <v>0.006604155901531289</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1825900803829362</v>
+        <v>0.1930457435224738</v>
       </c>
       <c r="G7" t="n">
-        <v>1.255123974637942</v>
+        <v>1.193795729666399</v>
       </c>
       <c r="H7" t="n">
-        <v>1.072967003262484</v>
+        <v>1.08071660018979</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>installment.rate.in.percentage.of.disposable.income</t>
+          <t>status.of.existing.checking.account</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.102622322228458</v>
+        <v>0.8466351865996518</v>
       </c>
       <c r="C8" t="n">
-        <v>0.5908922116896314</v>
+        <v>0.1270229592932462</v>
       </c>
       <c r="D8" t="n">
-        <v>1.866029540439458</v>
+        <v>6.665213842523563</v>
       </c>
       <c r="E8" t="n">
-        <v>0.06203723266238914</v>
+        <v>2.642802663818704e-11</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.05552641268321956</v>
+        <v>0.5976701863848892</v>
       </c>
       <c r="G8" t="n">
-        <v>2.260771057140135</v>
+        <v>1.095600186814414</v>
       </c>
       <c r="H8" t="n">
-        <v>1.025435550903797</v>
+        <v>1.10541631697432</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>present.employment.since</t>
+          <t>savings.account.and.bonds</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.7103598266956189</v>
+        <v>0.697840387314234</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2185851642251776</v>
+        <v>0.2745165520736341</v>
       </c>
       <c r="D9" t="n">
-        <v>3.249808051766198</v>
+        <v>2.542070348920349</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0011548292721742</v>
+        <v>0.01101979913215668</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2819329048142708</v>
+        <v>0.1597879452499112</v>
       </c>
       <c r="G9" t="n">
-        <v>1.138786748576967</v>
+        <v>1.235892829378557</v>
       </c>
       <c r="H9" t="n">
-        <v>1.044415019288108</v>
+        <v>1.063904865369559</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>purpose</t>
+          <t>age.in.years</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.8255836726156349</v>
+        <v>0.8766230693041976</v>
       </c>
       <c r="C10" t="n">
-        <v>0.3140191177994451</v>
+        <v>0.3562625415371521</v>
       </c>
       <c r="D10" t="n">
-        <v>2.629087293796269</v>
+        <v>2.460609710810085</v>
       </c>
       <c r="E10" t="n">
-        <v>0.008561438081778215</v>
+        <v>0.01387011580881202</v>
       </c>
       <c r="F10" t="n">
-        <v>0.2101062017287226</v>
+        <v>0.1783484878913796</v>
       </c>
       <c r="G10" t="n">
-        <v>1.441061143502547</v>
+        <v>1.574897650717016</v>
       </c>
       <c r="H10" t="n">
-        <v>1.031816977908369</v>
+        <v>1.074440820590449</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>credit.history</t>
+          <t>purpose</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.8365588769976238</v>
+        <v>0.9919068213366427</v>
       </c>
       <c r="C11" t="n">
-        <v>0.2155845987553848</v>
+        <v>0.2253459789141403</v>
       </c>
       <c r="D11" t="n">
-        <v>3.880420409561972</v>
+        <v>4.401706327826563</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0001042760645890972</v>
+        <v>1.074028652667904e-05</v>
       </c>
       <c r="F11" t="n">
-        <v>0.4140130634370696</v>
+        <v>0.5502287026649276</v>
       </c>
       <c r="G11" t="n">
-        <v>1.259104690558178</v>
+        <v>1.433584940008358</v>
       </c>
       <c r="H11" t="n">
-        <v>1.038474783996854</v>
-      </c>
-    </row>
-    <row r="12"/>
-    <row r="13"/>
+        <v>1.018799787099276</v>
+      </c>
+    </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
@@ -788,13 +788,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.7768014059753954</v>
+        <v>0.7876106194690266</v>
       </c>
       <c r="C16" t="n">
-        <v>0.9020408163265307</v>
+        <v>0.9081632653061225</v>
       </c>
       <c r="D16" t="n">
-        <v>0.8347497639282341</v>
+        <v>0.8436018957345971</v>
       </c>
       <c r="E16" t="n">
         <v>490</v>
@@ -807,13 +807,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.6335877862595419</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="C17" t="n">
-        <v>0.3952380952380952</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="D17" t="n">
-        <v>0.4868035190615835</v>
+        <v>0.5217391304347826</v>
       </c>
       <c r="E17" t="n">
         <v>210</v>
@@ -826,16 +826,16 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.75</v>
+        <v>0.7642857142857142</v>
       </c>
       <c r="C18" t="n">
-        <v>0.75</v>
+        <v>0.7642857142857142</v>
       </c>
       <c r="D18" t="n">
-        <v>0.75</v>
+        <v>0.7642857142857142</v>
       </c>
       <c r="E18" t="n">
-        <v>0.75</v>
+        <v>0.7642857142857142</v>
       </c>
     </row>
     <row r="19">
@@ -845,13 +845,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.7051945961174686</v>
+        <v>0.7271386430678466</v>
       </c>
       <c r="C19" t="n">
-        <v>0.648639455782313</v>
+        <v>0.6683673469387755</v>
       </c>
       <c r="D19" t="n">
-        <v>0.6607766414949088</v>
+        <v>0.6826705130846898</v>
       </c>
       <c r="E19" t="n">
         <v>700</v>
@@ -864,20 +864,18 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.7338373200606394</v>
+        <v>0.7513274336283186</v>
       </c>
       <c r="C20" t="n">
-        <v>0.75</v>
+        <v>0.7642857142857142</v>
       </c>
       <c r="D20" t="n">
-        <v>0.7303658904682389</v>
+        <v>0.7470430661446528</v>
       </c>
       <c r="E20" t="n">
         <v>700</v>
       </c>
     </row>
-    <row r="21"/>
-    <row r="22"/>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
@@ -919,13 +917,13 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.7878787878787878</v>
+        <v>0.7795918367346939</v>
       </c>
       <c r="C25" t="n">
-        <v>0.8666666666666667</v>
+        <v>0.9095238095238095</v>
       </c>
       <c r="D25" t="n">
-        <v>0.8253968253968254</v>
+        <v>0.8395604395604396</v>
       </c>
       <c r="E25" t="n">
         <v>210</v>
@@ -938,13 +936,13 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.5942028985507246</v>
+        <v>0.6545454545454545</v>
       </c>
       <c r="C26" t="n">
-        <v>0.4555555555555555</v>
+        <v>0.4</v>
       </c>
       <c r="D26" t="n">
-        <v>0.5157232704402516</v>
+        <v>0.496551724137931</v>
       </c>
       <c r="E26" t="n">
         <v>90</v>
@@ -957,16 +955,16 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.7433333333333333</v>
+        <v>0.7566666666666667</v>
       </c>
       <c r="C27" t="n">
-        <v>0.7433333333333333</v>
+        <v>0.7566666666666667</v>
       </c>
       <c r="D27" t="n">
-        <v>0.7433333333333333</v>
+        <v>0.7566666666666667</v>
       </c>
       <c r="E27" t="n">
-        <v>0.7433333333333333</v>
+        <v>0.7566666666666667</v>
       </c>
     </row>
     <row r="28">
@@ -976,13 +974,13 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.6910408432147562</v>
+        <v>0.7170686456400742</v>
       </c>
       <c r="C28" t="n">
-        <v>0.6611111111111111</v>
+        <v>0.6547619047619048</v>
       </c>
       <c r="D28" t="n">
-        <v>0.6705600479185385</v>
+        <v>0.6680560818491853</v>
       </c>
       <c r="E28" t="n">
         <v>300</v>
@@ -995,20 +993,18 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.7297760210803689</v>
+        <v>0.7420779220779221</v>
       </c>
       <c r="C29" t="n">
-        <v>0.7433333333333333</v>
+        <v>0.7566666666666667</v>
       </c>
       <c r="D29" t="n">
-        <v>0.7324947589098532</v>
+        <v>0.736657824933687</v>
       </c>
       <c r="E29" t="n">
         <v>300</v>
       </c>
     </row>
-    <row r="30"/>
-    <row r="31"/>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
@@ -1050,13 +1046,13 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.78</v>
+        <v>0.7851851851851852</v>
       </c>
       <c r="C34" t="n">
-        <v>0.8914285714285715</v>
+        <v>0.9085714285714286</v>
       </c>
       <c r="D34" t="n">
-        <v>0.8320000000000001</v>
+        <v>0.842384105960265</v>
       </c>
       <c r="E34" t="n">
         <v>700</v>
@@ -1069,13 +1065,13 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.62</v>
+        <v>0.6631578947368421</v>
       </c>
       <c r="C35" t="n">
-        <v>0.4133333333333333</v>
+        <v>0.42</v>
       </c>
       <c r="D35" t="n">
-        <v>0.496</v>
+        <v>0.5142857142857142</v>
       </c>
       <c r="E35" t="n">
         <v>300</v>
@@ -1088,16 +1084,16 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.748</v>
+        <v>0.762</v>
       </c>
       <c r="C36" t="n">
-        <v>0.748</v>
+        <v>0.762</v>
       </c>
       <c r="D36" t="n">
-        <v>0.748</v>
+        <v>0.762</v>
       </c>
       <c r="E36" t="n">
-        <v>0.748</v>
+        <v>0.762</v>
       </c>
     </row>
     <row r="37">
@@ -1107,13 +1103,13 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.7</v>
+        <v>0.7241715399610136</v>
       </c>
       <c r="C37" t="n">
-        <v>0.6523809523809524</v>
+        <v>0.6642857142857143</v>
       </c>
       <c r="D37" t="n">
-        <v>0.664</v>
+        <v>0.6783349101229896</v>
       </c>
       <c r="E37" t="n">
         <v>1000</v>
@@ -1126,13 +1122,13 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.732</v>
+        <v>0.7485769980506822</v>
       </c>
       <c r="C38" t="n">
-        <v>0.748</v>
+        <v>0.762</v>
       </c>
       <c r="D38" t="n">
-        <v>0.7312000000000001</v>
+        <v>0.7439545884578997</v>
       </c>
       <c r="E38" t="n">
         <v>1000</v>
@@ -1144,6 +1140,1269 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:I34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="53" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="53" customWidth="1" min="3" max="3"/>
+    <col width="24" customWidth="1" min="4" max="4"/>
+    <col width="24" customWidth="1" min="5" max="5"/>
+    <col width="38" customWidth="1" min="6" max="6"/>
+    <col width="28" customWidth="1" min="7" max="7"/>
+    <col width="24" customWidth="1" min="8" max="8"/>
+    <col width="24" customWidth="1" min="9" max="9"/>
+  </cols>
+  <sheetData>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>训练数据集入模变量相关性</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>credit.amount</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>installment.rate.in.percentage.of.disposable.income</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>housing</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>credit.history</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>status.of.existing.checking.account</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>savings.account.and.bonds</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>age.in.years</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>purpose</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>credit.amount</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-0.2384425532969876</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.08556969316697344</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.02684241826093913</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.1020048297900735</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0001902234863647554</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-0.01437342321663895</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.06613843488262584</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>installment.rate.in.percentage.of.disposable.income</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-0.2384425532969876</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-0.0393887944855453</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-0.0488358679775112</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-0.02837242993620628</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-0.0704805779741953</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-0.04749736367166204</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.002980775936174611</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>housing</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.08556969316697344</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-0.0393887944855453</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.06872137691470744</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.1520705026393233</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.04223962573541496</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-0.007932068382037645</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.01443171488504034</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>credit.history</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.02684241826093913</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-0.0488358679775112</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.06872137691470744</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.1738301558933878</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.03874349560174618</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.2103751231754975</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.01865324567659059</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>status.of.existing.checking.account</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.1020048297900735</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-0.02837242993620628</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.1520705026393233</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.1738301558933878</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.1964816657547299</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.05894110741143806</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.07709145662727833</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>savings.account.and.bonds</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.0001902234863647554</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-0.0704805779741953</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.04223962573541496</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.03874349560174618</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.1964816657547299</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.1320016687743047</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.04190695091725297</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>age.in.years</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-0.01437342321663895</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-0.04749736367166204</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-0.007932068382037645</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.2103751231754975</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.05894110741143806</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.1320016687743047</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>-0.07825690646384501</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>purpose</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.06613843488262584</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.002980775936174611</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.01443171488504034</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.01865324567659059</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.07709145662727833</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.04190695091725297</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-0.07825690646384501</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>测试数据集入模变量相关性</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>credit.amount</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>installment.rate.in.percentage.of.disposable.income</t>
+        </is>
+      </c>
+      <c r="D14" s="1" t="inlineStr">
+        <is>
+          <t>housing</t>
+        </is>
+      </c>
+      <c r="E14" s="1" t="inlineStr">
+        <is>
+          <t>credit.history</t>
+        </is>
+      </c>
+      <c r="F14" s="1" t="inlineStr">
+        <is>
+          <t>status.of.existing.checking.account</t>
+        </is>
+      </c>
+      <c r="G14" s="1" t="inlineStr">
+        <is>
+          <t>savings.account.and.bonds</t>
+        </is>
+      </c>
+      <c r="H14" s="1" t="inlineStr">
+        <is>
+          <t>age.in.years</t>
+        </is>
+      </c>
+      <c r="I14" s="1" t="inlineStr">
+        <is>
+          <t>purpose</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>credit.amount</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-0.2008406921589413</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.08354204883175859</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-0.006601275780911853</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-0.0005555629283977131</v>
+      </c>
+      <c r="G15" t="n">
+        <v>-0.02548766373991636</v>
+      </c>
+      <c r="H15" t="n">
+        <v>-0.05066539072070925</v>
+      </c>
+      <c r="I15" t="n">
+        <v>-0.02586924932274625</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>installment.rate.in.percentage.of.disposable.income</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>-0.2008406921589413</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-0.07785683383715965</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-0.02496272889984229</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.1273324983438082</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.003456978125794201</v>
+      </c>
+      <c r="H16" t="n">
+        <v>-0.03455716777210553</v>
+      </c>
+      <c r="I16" t="n">
+        <v>-0.02452980911122184</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>housing</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.08354204883175859</v>
+      </c>
+      <c r="C17" t="n">
+        <v>-0.07785683383715965</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.1113812485997314</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.06398584317078343</v>
+      </c>
+      <c r="G17" t="n">
+        <v>-0.06025949090780384</v>
+      </c>
+      <c r="H17" t="n">
+        <v>-0.001724826266999777</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.008751750525175066</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>credit.history</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>-0.006601275780911853</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-0.02496272889984229</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.1113812485997314</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.1010472075260841</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.01749513484208905</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.08789683339733805</v>
+      </c>
+      <c r="I18" t="n">
+        <v>-0.05517372590682453</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>status.of.existing.checking.account</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>-0.0005555629283977131</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.1273324983438082</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.06398584317078343</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.1010472075260841</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.2698678084343024</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.1271306419259191</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.04943903067392558</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>savings.account.and.bonds</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>-0.02548766373991636</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.003456978125794201</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-0.06025949090780384</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.01749513484208905</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.2698678084343024</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.1641696445040569</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.03019921694445682</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>age.in.years</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-0.05066539072070925</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-0.03455716777210553</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-0.001724826266999777</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.08789683339733805</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.1271306419259191</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.1641696445040569</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>-0.1286517770800275</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>purpose</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>-0.02586924932274625</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-0.02452980911122184</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.008751750525175066</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-0.05517372590682453</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.04943903067392558</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.03019921694445682</v>
+      </c>
+      <c r="H22" t="n">
+        <v>-0.1286517770800275</v>
+      </c>
+      <c r="I22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>跨时间验证集入模变量相关性</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>credit.amount</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>installment.rate.in.percentage.of.disposable.income</t>
+        </is>
+      </c>
+      <c r="D26" s="1" t="inlineStr">
+        <is>
+          <t>housing</t>
+        </is>
+      </c>
+      <c r="E26" s="1" t="inlineStr">
+        <is>
+          <t>credit.history</t>
+        </is>
+      </c>
+      <c r="F26" s="1" t="inlineStr">
+        <is>
+          <t>status.of.existing.checking.account</t>
+        </is>
+      </c>
+      <c r="G26" s="1" t="inlineStr">
+        <is>
+          <t>savings.account.and.bonds</t>
+        </is>
+      </c>
+      <c r="H26" s="1" t="inlineStr">
+        <is>
+          <t>age.in.years</t>
+        </is>
+      </c>
+      <c r="I26" s="1" t="inlineStr">
+        <is>
+          <t>purpose</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>credit.amount</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-0.2271478957618095</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.08255162949771064</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.01592872700126408</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.07120749721408075</v>
+      </c>
+      <c r="G27" t="n">
+        <v>-0.007806314583802167</v>
+      </c>
+      <c r="H27" t="n">
+        <v>-0.02510258972040505</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.04138877325745291</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>installment.rate.in.percentage.of.disposable.income</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>-0.2271478957618095</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" t="n">
+        <v>-0.05139870701340384</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-0.04193449301022911</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.0186045453370852</v>
+      </c>
+      <c r="G28" t="n">
+        <v>-0.04859067078372906</v>
+      </c>
+      <c r="H28" t="n">
+        <v>-0.04364364957077333</v>
+      </c>
+      <c r="I28" t="n">
+        <v>-0.005068085821911168</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>housing</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.08255162949771064</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-0.05139870701340384</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.08301149661073569</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.1253481720816791</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.01153852037432568</v>
+      </c>
+      <c r="H29" t="n">
+        <v>-0.005667681861715859</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.01095383890169336</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>credit.history</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.01592872700126408</v>
+      </c>
+      <c r="C30" t="n">
+        <v>-0.04193449301022911</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.08301149661073569</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.1528682006259729</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.03307333180955983</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.1746614975428908</v>
+      </c>
+      <c r="I30" t="n">
+        <v>-0.003948816888179707</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>status.of.existing.checking.account</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0.07120749721408075</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.0186045453370852</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.1253481720816791</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.1528682006259729</v>
+      </c>
+      <c r="F31" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.2186454598230806</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.07965074442732671</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.06803460242361524</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>savings.account.and.bonds</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>-0.007806314583802167</v>
+      </c>
+      <c r="C32" t="n">
+        <v>-0.04859067078372906</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.01153852037432568</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.03307333180955983</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.2186454598230806</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.141622365072126</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.03788688382273341</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>age.in.years</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>-0.02510258972040505</v>
+      </c>
+      <c r="C33" t="n">
+        <v>-0.04364364957077333</v>
+      </c>
+      <c r="D33" t="n">
+        <v>-0.005667681861715859</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.1746614975428908</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.07965074442732671</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.141622365072126</v>
+      </c>
+      <c r="H33" t="n">
+        <v>1</v>
+      </c>
+      <c r="I33" t="n">
+        <v>-0.09341175999911115</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>purpose</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0.04138877325745291</v>
+      </c>
+      <c r="C34" t="n">
+        <v>-0.005068085821911168</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.01095383890169336</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-0.003948816888179707</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.06803460242361524</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.03788688382273341</v>
+      </c>
+      <c r="H34" t="n">
+        <v>-0.09341175999911115</v>
+      </c>
+      <c r="I34" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13" customWidth="1" min="1" max="1"/>
+    <col width="53" customWidth="1" min="2" max="2"/>
+    <col width="53" customWidth="1" min="3" max="3"/>
+    <col width="9" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>score</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>credit.amount</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>[-inf ~ 3914)</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>85.14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>credit.amount</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>[3914 ~ inf)</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>16.31</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>installment.rate.in.percentage.of.disposable.income</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>[-inf ~ 4)</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>90.19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>installment.rate.in.percentage.of.disposable.income</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>[4 ~ inf)</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>38.23</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>housing</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>own</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>74.84999999999999</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>housing</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>for free,rent</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>39.7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>credit.history</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>critical account/ other credits existing (not at this bank)</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>102.98</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>credit.history</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>existing credits paid back duly till now,delay in paying off in the past,all credits at this bank paid back duly,no credits taken/ all credits paid back duly</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>50.61</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>status.of.existing.checking.account</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>no checking account,... &gt;= 200 DM / salary assignments for at least 1 year</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>133.9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>status.of.existing.checking.account</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0 &lt;= ... &lt; 200 DM</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>38.14</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>status.of.existing.checking.account</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>... &lt; 0 DM</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>savings.account.and.bonds</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>... &gt;= 1000 DM,500 &lt;= ... &lt; 1000 DM,unknown/ no savings account</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>100.29</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>savings.account.and.bonds</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>100 &lt;= ... &lt; 500 DM,... &lt; 100 DM</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>51.64</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>age.in.years</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>[-inf ~ 35)</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>46.84</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>age.in.years</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>[35 ~ inf)</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>88.01000000000001</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>purpose</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>car (used),retraining,radio/television,furniture/equipment</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>98.39</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>purpose</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>business,repairs,domestic appliances,others,car (new),education</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>27.42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1161,16 +2420,16 @@
     <col width="13" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
     <col width="13" customWidth="1" min="6" max="6"/>
-    <col width="22" customWidth="1" min="7" max="7"/>
+    <col width="23" customWidth="1" min="7" max="7"/>
     <col width="13" customWidth="1" min="8" max="8"/>
     <col width="23" customWidth="1" min="9" max="9"/>
     <col width="22" customWidth="1" min="10" max="10"/>
     <col width="22" customWidth="1" min="11" max="11"/>
     <col width="23" customWidth="1" min="12" max="12"/>
     <col width="20" customWidth="1" min="13" max="13"/>
-    <col width="22" customWidth="1" min="14" max="14"/>
+    <col width="21" customWidth="1" min="14" max="14"/>
     <col width="20" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
@@ -1275,16 +2534,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1</v>
+        <v>0.09857142857142857</v>
       </c>
       <c r="F3" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" t="n">
-        <v>0.04081632653061224</v>
+        <v>0.03877551020408163</v>
       </c>
       <c r="H3" t="n">
         <v>50</v>
@@ -1293,22 +2552,22 @@
         <v>0.2380952380952381</v>
       </c>
       <c r="J3" t="n">
-        <v>0.7142857142857143</v>
+        <v>0.7246376811594203</v>
       </c>
       <c r="K3" t="n">
-        <v>-1.763592792252539</v>
+        <v>-1.814886086640089</v>
       </c>
       <c r="L3" t="n">
-        <v>0.3479196664988001</v>
+        <v>0.3617426009425483</v>
       </c>
       <c r="M3" t="n">
-        <v>1.787473590767906</v>
+        <v>1.256123789263948</v>
       </c>
       <c r="N3" t="n">
-        <v>2.380952380952381</v>
+        <v>2.415458937198068</v>
       </c>
       <c r="O3" t="n">
-        <v>2.380952380952381</v>
+        <v>2.415458937198068</v>
       </c>
     </row>
     <row r="4">
@@ -1328,40 +2587,40 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E4" t="n">
-        <v>0.11</v>
+        <v>0.1028571428571429</v>
       </c>
       <c r="F4" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G4" t="n">
-        <v>0.07551020408163266</v>
+        <v>0.06326530612244897</v>
       </c>
       <c r="H4" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1904761904761905</v>
+        <v>0.1952380952380952</v>
       </c>
       <c r="J4" t="n">
-        <v>0.5194805194805194</v>
+        <v>0.5694444444444444</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.9252646518431341</v>
+        <v>-1.126887844544468</v>
       </c>
       <c r="L4" t="n">
-        <v>0.106373963375163</v>
+        <v>0.1487185318650522</v>
       </c>
       <c r="M4" t="n">
-        <v>1.787473590767906</v>
+        <v>1.256123789263948</v>
       </c>
       <c r="N4" t="n">
-        <v>1.731601731601732</v>
+        <v>1.898148148148148</v>
       </c>
       <c r="O4" t="n">
-        <v>4.112554112554113</v>
+        <v>4.313607085346216</v>
       </c>
     </row>
     <row r="5">
@@ -1381,40 +2640,40 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1614285714285714</v>
+        <v>0.1714285714285714</v>
       </c>
       <c r="F5" t="n">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1163265306122449</v>
+        <v>0.1387755102040816</v>
       </c>
       <c r="H5" t="n">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I5" t="n">
-        <v>0.2666666666666667</v>
+        <v>0.2476190476190476</v>
       </c>
       <c r="J5" t="n">
-        <v>0.495575221238938</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.8296020332807714</v>
+        <v>-0.5790379122459083</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1247224825544561</v>
+        <v>0.06302453466622132</v>
       </c>
       <c r="M5" t="n">
-        <v>1.787473590767906</v>
+        <v>1.256123789263948</v>
       </c>
       <c r="N5" t="n">
-        <v>1.651917404129793</v>
+        <v>1.444444444444445</v>
       </c>
       <c r="O5" t="n">
-        <v>5.764471516683907</v>
+        <v>5.75805152979066</v>
       </c>
     </row>
     <row r="6">
@@ -1434,16 +2693,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1871428571428571</v>
+        <v>0.1842857142857143</v>
       </c>
       <c r="F6" t="n">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G6" t="n">
-        <v>0.2061224489795918</v>
+        <v>0.2020408163265306</v>
       </c>
       <c r="H6" t="n">
         <v>30</v>
@@ -1452,22 +2711,22 @@
         <v>0.1428571428571428</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2290076335877863</v>
+        <v>0.2325581395348837</v>
       </c>
       <c r="K6" t="n">
-        <v>0.3666182748164004</v>
+        <v>0.3466176081097309</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0231942173863437</v>
+        <v>0.02051410333710653</v>
       </c>
       <c r="M6" t="n">
-        <v>1.787473590767906</v>
+        <v>1.256123789263948</v>
       </c>
       <c r="N6" t="n">
-        <v>0.7633587786259542</v>
+        <v>0.7751937984496124</v>
       </c>
       <c r="O6" t="n">
-        <v>6.527830295309861</v>
+        <v>6.533245328240273</v>
       </c>
     </row>
     <row r="7">
@@ -1487,40 +2746,40 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1614285714285714</v>
+        <v>0.1657142857142857</v>
       </c>
       <c r="F7" t="n">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1857142857142857</v>
+        <v>0.1897959183673469</v>
       </c>
       <c r="H7" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I7" t="n">
-        <v>0.1047619047619048</v>
+        <v>0.1095238095238095</v>
       </c>
       <c r="J7" t="n">
-        <v>0.1946902654867257</v>
+        <v>0.1982758620689655</v>
       </c>
       <c r="K7" t="n">
-        <v>0.5725096473623428</v>
+        <v>0.5497982864438022</v>
       </c>
       <c r="L7" t="n">
-        <v>0.04634601907218965</v>
+        <v>0.04413346789140726</v>
       </c>
       <c r="M7" t="n">
-        <v>1.787473590767906</v>
+        <v>1.256123789263948</v>
       </c>
       <c r="N7" t="n">
-        <v>0.6489675516224189</v>
+        <v>0.6609195402298851</v>
       </c>
       <c r="O7" t="n">
-        <v>7.17679784693228</v>
+        <v>7.194164868470159</v>
       </c>
     </row>
     <row r="8">
@@ -1540,40 +2799,40 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1214285714285714</v>
+        <v>0.1242857142857143</v>
       </c>
       <c r="F8" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1571428571428571</v>
+        <v>0.1591836734693877</v>
       </c>
       <c r="H8" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0380952380952381</v>
+        <v>0.04285714285714286</v>
       </c>
       <c r="J8" t="n">
-        <v>0.09411764705882353</v>
+        <v>0.103448275862069</v>
       </c>
       <c r="K8" t="n">
-        <v>1.417039770131169</v>
+        <v>1.312163055905053</v>
       </c>
       <c r="L8" t="n">
-        <v>0.1686952107299011</v>
+        <v>0.152639375890996</v>
       </c>
       <c r="M8" t="n">
-        <v>1.787473590767906</v>
+        <v>1.256123789263948</v>
       </c>
       <c r="N8" t="n">
-        <v>0.3137254901960784</v>
+        <v>0.3448275862068966</v>
       </c>
       <c r="O8" t="n">
-        <v>7.490523337128358</v>
+        <v>7.538992454677055</v>
       </c>
     </row>
     <row r="9">
@@ -1593,40 +2852,40 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1085714285714286</v>
+        <v>0.09714285714285714</v>
       </c>
       <c r="F9" t="n">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G9" t="n">
-        <v>0.1510204081632653</v>
+        <v>0.1326530612244898</v>
       </c>
       <c r="H9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I9" t="n">
-        <v>0.009523809523809525</v>
+        <v>0.01428571428571429</v>
       </c>
       <c r="J9" t="n">
-        <v>0.02631578947368421</v>
+        <v>0.04411764705882353</v>
       </c>
       <c r="K9" t="n">
-        <v>2.763515057769135</v>
+        <v>2.228407123290209</v>
       </c>
       <c r="L9" t="n">
-        <v>0.3910279809632518</v>
+        <v>0.2637706390833309</v>
       </c>
       <c r="M9" t="n">
-        <v>1.787473590767906</v>
+        <v>1.256123789263948</v>
       </c>
       <c r="N9" t="n">
-        <v>0.08771929824561403</v>
+        <v>0.1470588235294118</v>
       </c>
       <c r="O9" t="n">
-        <v>7.578242635373972</v>
+        <v>7.686051278206468</v>
       </c>
     </row>
     <row r="10">
@@ -1646,40 +2905,40 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="E10" t="n">
-        <v>0.03714285714285714</v>
+        <v>0.04857142857142857</v>
       </c>
       <c r="F10" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G10" t="n">
-        <v>0.05306122448979592</v>
+        <v>0.0653061224489796</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>0.009523809523809525</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="K10" t="n">
-        <v>10.87920170488108</v>
+        <v>1.925185867364692</v>
       </c>
       <c r="L10" t="n">
-        <v>0.5772637639324656</v>
+        <v>0.1073913204924522</v>
       </c>
       <c r="M10" t="n">
-        <v>1.787473590767906</v>
+        <v>1.256123789263948</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>0.196078431372549</v>
       </c>
       <c r="O10" t="n">
-        <v>7.578242635373972</v>
+        <v>7.882129709579017</v>
       </c>
     </row>
     <row r="11">
@@ -1699,44 +2958,42 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E11" t="n">
-        <v>0.01285714285714286</v>
+        <v>0.007142857142857143</v>
       </c>
       <c r="F11" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G11" t="n">
-        <v>0.01428571428571429</v>
+        <v>0.01020408163265306</v>
       </c>
       <c r="H11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0.009523809523809525</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>0.2222222222222222</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>0.4053601136202785</v>
+        <v>9.230543079293701</v>
       </c>
       <c r="L11" t="n">
-        <v>0.001930286255334659</v>
+        <v>0.09418921509483368</v>
       </c>
       <c r="M11" t="n">
-        <v>1.787473590767906</v>
+        <v>1.256123789263948</v>
       </c>
       <c r="N11" t="n">
-        <v>0.7407407407407407</v>
+        <v>0</v>
       </c>
       <c r="O11" t="n">
-        <v>8.318983376114712</v>
-      </c>
-    </row>
-    <row r="12"/>
-    <row r="13"/>
+        <v>7.882129709579017</v>
+      </c>
+    </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
@@ -1838,40 +3095,40 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E16" t="n">
-        <v>0.1133333333333333</v>
+        <v>0.09333333333333334</v>
       </c>
       <c r="F16" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G16" t="n">
-        <v>0.05238095238095238</v>
+        <v>0.04761904761904762</v>
       </c>
       <c r="H16" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I16" t="n">
-        <v>0.2555555555555555</v>
+        <v>0.2</v>
       </c>
       <c r="J16" t="n">
-        <v>0.6764705882352942</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="K16" t="n">
-        <v>-1.584900716553805</v>
+        <v>-1.435089525276823</v>
       </c>
       <c r="L16" t="n">
-        <v>0.3220115741569635</v>
+        <v>0.2186803086136111</v>
       </c>
       <c r="M16" t="n">
-        <v>2.084586230255282</v>
+        <v>3.072899861866642</v>
       </c>
       <c r="N16" t="n">
-        <v>2.254901960784314</v>
+        <v>2.142857142857143</v>
       </c>
       <c r="O16" t="n">
-        <v>2.254901960784314</v>
+        <v>2.142857142857143</v>
       </c>
     </row>
     <row r="17">
@@ -1891,16 +3148,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="E17" t="n">
-        <v>0.1433333333333333</v>
+        <v>0.1066666666666667</v>
       </c>
       <c r="F17" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="G17" t="n">
-        <v>0.1047619047619048</v>
+        <v>0.05238095238095238</v>
       </c>
       <c r="H17" t="n">
         <v>21</v>
@@ -1909,22 +3166,22 @@
         <v>0.2333333333333333</v>
       </c>
       <c r="J17" t="n">
-        <v>0.4883720930232558</v>
+        <v>0.65625</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.8007821304574129</v>
+        <v>-1.493929311017358</v>
       </c>
       <c r="L17" t="n">
-        <v>0.1029577024873816</v>
+        <v>0.270330065803141</v>
       </c>
       <c r="M17" t="n">
-        <v>2.084586230255282</v>
+        <v>3.072899861866642</v>
       </c>
       <c r="N17" t="n">
-        <v>1.627906976744186</v>
+        <v>2.1875</v>
       </c>
       <c r="O17" t="n">
-        <v>3.8828089375285</v>
+        <v>4.330357142857143</v>
       </c>
     </row>
     <row r="18">
@@ -1944,40 +3201,40 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E18" t="n">
-        <v>0.14</v>
+        <v>0.1766666666666667</v>
       </c>
       <c r="F18" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G18" t="n">
-        <v>0.1142857142857143</v>
+        <v>0.1523809523809524</v>
       </c>
       <c r="H18" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I18" t="n">
-        <v>0.2</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="J18" t="n">
-        <v>0.4285714285714285</v>
+        <v>0.3962264150943396</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.5596207879229228</v>
+        <v>-0.4260886810160021</v>
       </c>
       <c r="L18" t="n">
-        <v>0.04796749610767911</v>
+        <v>0.03449289322510492</v>
       </c>
       <c r="M18" t="n">
-        <v>2.084586230255282</v>
+        <v>3.072899861866642</v>
       </c>
       <c r="N18" t="n">
-        <v>1.428571428571429</v>
+        <v>1.320754716981132</v>
       </c>
       <c r="O18" t="n">
-        <v>5.311380366099929</v>
+        <v>5.651111859838275</v>
       </c>
     </row>
     <row r="19">
@@ -1997,40 +3254,40 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E19" t="n">
-        <v>0.17</v>
+        <v>0.1866666666666667</v>
       </c>
       <c r="F19" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G19" t="n">
-        <v>0.1809523809523809</v>
+        <v>0.1761904761904762</v>
       </c>
       <c r="H19" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="I19" t="n">
-        <v>0.1444444444444444</v>
+        <v>0.2111111111111111</v>
       </c>
       <c r="J19" t="n">
-        <v>0.2549019607843137</v>
+        <v>0.3392857142857143</v>
       </c>
       <c r="K19" t="n">
-        <v>0.2253320188246868</v>
+        <v>-0.1808236637403061</v>
       </c>
       <c r="L19" t="n">
-        <v>0.008226407036456823</v>
+        <v>0.006314477146486877</v>
       </c>
       <c r="M19" t="n">
-        <v>2.084586230255282</v>
+        <v>3.072899861866642</v>
       </c>
       <c r="N19" t="n">
-        <v>0.8496732026143791</v>
+        <v>1.130952380952381</v>
       </c>
       <c r="O19" t="n">
-        <v>6.161053568714308</v>
+        <v>6.782064240790657</v>
       </c>
     </row>
     <row r="20">
@@ -2050,16 +3307,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E20" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.15</v>
       </c>
       <c r="F20" t="n">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G20" t="n">
-        <v>0.2</v>
+        <v>0.1761904761904762</v>
       </c>
       <c r="H20" t="n">
         <v>8</v>
@@ -2068,22 +3325,22 @@
         <v>0.08888888888888889</v>
       </c>
       <c r="J20" t="n">
-        <v>0.16</v>
+        <v>0.1777777777777778</v>
       </c>
       <c r="K20" t="n">
-        <v>0.8109189662796096</v>
+        <v>0.6841672606404656</v>
       </c>
       <c r="L20" t="n">
-        <v>0.09010210736440107</v>
+        <v>0.05972888783369145</v>
       </c>
       <c r="M20" t="n">
-        <v>2.084586230255282</v>
+        <v>3.072899861866642</v>
       </c>
       <c r="N20" t="n">
-        <v>0.5333333333333333</v>
+        <v>0.5925925925925927</v>
       </c>
       <c r="O20" t="n">
-        <v>6.694386902047641</v>
+        <v>7.374656833383249</v>
       </c>
     </row>
     <row r="21">
@@ -2103,40 +3360,40 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E21" t="n">
-        <v>0.14</v>
+        <v>0.1533333333333333</v>
       </c>
       <c r="F21" t="n">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="G21" t="n">
-        <v>0.1714285714285714</v>
+        <v>0.2047619047619048</v>
       </c>
       <c r="H21" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I21" t="n">
-        <v>0.06666666666666667</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="J21" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.06521739130434782</v>
       </c>
       <c r="K21" t="n">
-        <v>0.9444466089533502</v>
+        <v>1.81525996708824</v>
       </c>
       <c r="L21" t="n">
-        <v>0.09894202569987479</v>
+        <v>0.3111874229294126</v>
       </c>
       <c r="M21" t="n">
-        <v>2.084586230255282</v>
+        <v>3.072899861866642</v>
       </c>
       <c r="N21" t="n">
-        <v>0.4761904761904762</v>
+        <v>0.2173913043478261</v>
       </c>
       <c r="O21" t="n">
-        <v>7.170577378238117</v>
+        <v>7.592048137731076</v>
       </c>
     </row>
     <row r="22">
@@ -2156,16 +3413,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E22" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="F22" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G22" t="n">
-        <v>0.1</v>
+        <v>0.119047619047619</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -2177,19 +3434,19 @@
         <v>0</v>
       </c>
       <c r="K22" t="n">
-        <v>11.51292546497023</v>
+        <v>11.68727885211501</v>
       </c>
       <c r="L22" t="n">
-        <v>1.151292546497023</v>
+        <v>1.391342720489882</v>
       </c>
       <c r="M22" t="n">
-        <v>2.084586230255282</v>
+        <v>3.072899861866642</v>
       </c>
       <c r="N22" t="n">
         <v>0</v>
       </c>
       <c r="O22" t="n">
-        <v>7.170577378238117</v>
+        <v>7.592048137731076</v>
       </c>
     </row>
     <row r="23">
@@ -2209,40 +3466,40 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E23" t="n">
-        <v>0.04333333333333333</v>
+        <v>0.04666666666666667</v>
       </c>
       <c r="F23" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G23" t="n">
-        <v>0.05714285714285714</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="H23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>0.01111111111111111</v>
+        <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>0.07692307692307693</v>
+        <v>0</v>
       </c>
       <c r="K23" t="n">
-        <v>1.637518793450554</v>
+        <v>11.10746035686206</v>
       </c>
       <c r="L23" t="n">
-        <v>0.07537784922232707</v>
+        <v>0.7404973571241377</v>
       </c>
       <c r="M23" t="n">
-        <v>2.084586230255282</v>
+        <v>3.072899861866642</v>
       </c>
       <c r="N23" t="n">
-        <v>0.2564102564102564</v>
+        <v>0</v>
       </c>
       <c r="O23" t="n">
-        <v>7.426987634648373</v>
+        <v>7.592048137731076</v>
       </c>
     </row>
     <row r="24">
@@ -2262,16 +3519,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E24" t="n">
-        <v>0.01333333333333333</v>
+        <v>0.003333333333333334</v>
       </c>
       <c r="F24" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G24" t="n">
-        <v>0.01904761904761905</v>
+        <v>0.004761904761904762</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -2283,23 +3540,21 @@
         <v>0</v>
       </c>
       <c r="K24" t="n">
-        <v>9.854697388366697</v>
+        <v>8.468403027246806</v>
       </c>
       <c r="L24" t="n">
-        <v>0.1877085216831752</v>
+        <v>0.04032572870117527</v>
       </c>
       <c r="M24" t="n">
-        <v>2.084586230255282</v>
+        <v>3.072899861866642</v>
       </c>
       <c r="N24" t="n">
         <v>0</v>
       </c>
       <c r="O24" t="n">
-        <v>7.426987634648373</v>
-      </c>
-    </row>
-    <row r="25"/>
-    <row r="26"/>
+        <v>7.592048137731076</v>
+      </c>
+    </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
@@ -2401,40 +3656,40 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E29" t="n">
-        <v>0.104</v>
+        <v>0.097</v>
       </c>
       <c r="F29" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G29" t="n">
-        <v>0.04428571428571428</v>
+        <v>0.04142857142857143</v>
       </c>
       <c r="H29" t="n">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I29" t="n">
-        <v>0.2433333333333333</v>
+        <v>0.2266666666666667</v>
       </c>
       <c r="J29" t="n">
-        <v>0.7019230769230769</v>
+        <v>0.7010309278350515</v>
       </c>
       <c r="K29" t="n">
-        <v>-1.703774206631045</v>
+        <v>-1.69951414733181</v>
       </c>
       <c r="L29" t="n">
-        <v>0.3391321992246557</v>
+        <v>0.3148147634819401</v>
       </c>
       <c r="M29" t="n">
-        <v>1.300052983403203</v>
+        <v>1.313366602419445</v>
       </c>
       <c r="N29" t="n">
-        <v>2.33974358974359</v>
+        <v>2.336769759450172</v>
       </c>
       <c r="O29" t="n">
-        <v>2.33974358974359</v>
+        <v>2.336769759450172</v>
       </c>
     </row>
     <row r="30">
@@ -2454,40 +3709,40 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="E30" t="n">
-        <v>0.12</v>
+        <v>0.104</v>
       </c>
       <c r="F30" t="n">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="G30" t="n">
-        <v>0.08428571428571428</v>
+        <v>0.06</v>
       </c>
       <c r="H30" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I30" t="n">
-        <v>0.2033333333333333</v>
+        <v>0.2066666666666667</v>
       </c>
       <c r="J30" t="n">
-        <v>0.5083333333333333</v>
+        <v>0.5961538461538461</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.8806391986754888</v>
+        <v>-1.236767465846898</v>
       </c>
       <c r="L30" t="n">
-        <v>0.1048379998423201</v>
+        <v>0.181392561657545</v>
       </c>
       <c r="M30" t="n">
-        <v>1.300052983403203</v>
+        <v>1.313366602419445</v>
       </c>
       <c r="N30" t="n">
-        <v>1.694444444444444</v>
+        <v>1.987179487179487</v>
       </c>
       <c r="O30" t="n">
-        <v>4.034188034188034</v>
+        <v>4.32394924662966</v>
       </c>
     </row>
     <row r="31">
@@ -2507,40 +3762,40 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="E31" t="n">
-        <v>0.155</v>
+        <v>0.173</v>
       </c>
       <c r="F31" t="n">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="G31" t="n">
-        <v>0.1157142857142857</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="H31" t="n">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I31" t="n">
-        <v>0.2466666666666667</v>
+        <v>0.2433333333333333</v>
       </c>
       <c r="J31" t="n">
-        <v>0.4774193548387097</v>
+        <v>0.4219653179190752</v>
       </c>
       <c r="K31" t="n">
-        <v>-0.756917852964771</v>
+        <v>-0.5325912251281003</v>
       </c>
       <c r="L31" t="n">
-        <v>0.09912019503110096</v>
+        <v>0.05351273738191866</v>
       </c>
       <c r="M31" t="n">
-        <v>1.300052983403203</v>
+        <v>1.313366602419445</v>
       </c>
       <c r="N31" t="n">
-        <v>1.591397849462366</v>
+        <v>1.406551059730251</v>
       </c>
       <c r="O31" t="n">
-        <v>5.6255858836504</v>
+        <v>5.73050030635991</v>
       </c>
     </row>
     <row r="32">
@@ -2560,40 +3815,40 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E32" t="n">
-        <v>0.182</v>
+        <v>0.185</v>
       </c>
       <c r="F32" t="n">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G32" t="n">
-        <v>0.1985714285714286</v>
+        <v>0.1942857142857143</v>
       </c>
       <c r="H32" t="n">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="I32" t="n">
-        <v>0.1433333333333333</v>
+        <v>0.1633333333333333</v>
       </c>
       <c r="J32" t="n">
-        <v>0.2362637362637363</v>
+        <v>0.2648648648648649</v>
       </c>
       <c r="K32" t="n">
-        <v>0.3259689803300769</v>
+        <v>0.1735306048079843</v>
       </c>
       <c r="L32" t="n">
-        <v>0.01800590558013758</v>
+        <v>0.0053711853869138</v>
       </c>
       <c r="M32" t="n">
-        <v>1.300052983403203</v>
+        <v>1.313366602419445</v>
       </c>
       <c r="N32" t="n">
-        <v>0.7875457875457875</v>
+        <v>0.882882882882883</v>
       </c>
       <c r="O32" t="n">
-        <v>6.413131671196187</v>
+        <v>6.613383189242793</v>
       </c>
     </row>
     <row r="33">
@@ -2613,40 +3868,40 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E33" t="n">
-        <v>0.163</v>
+        <v>0.161</v>
       </c>
       <c r="F33" t="n">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G33" t="n">
-        <v>0.19</v>
+        <v>0.1857142857142857</v>
       </c>
       <c r="H33" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I33" t="n">
-        <v>0.1</v>
+        <v>0.1033333333333333</v>
       </c>
       <c r="J33" t="n">
-        <v>0.1840490797546012</v>
+        <v>0.1925465838509317</v>
       </c>
       <c r="K33" t="n">
-        <v>0.6418438862223944</v>
+        <v>0.5862397082107037</v>
       </c>
       <c r="L33" t="n">
-        <v>0.05776594976001549</v>
+        <v>0.04829498548592941</v>
       </c>
       <c r="M33" t="n">
-        <v>1.300052983403203</v>
+        <v>1.313366602419445</v>
       </c>
       <c r="N33" t="n">
-        <v>0.6134969325153374</v>
+        <v>0.6418219461697723</v>
       </c>
       <c r="O33" t="n">
-        <v>7.026628603711525</v>
+        <v>7.255205135412565</v>
       </c>
     </row>
     <row r="34">
@@ -2666,40 +3921,40 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E34" t="n">
-        <v>0.127</v>
+        <v>0.133</v>
       </c>
       <c r="F34" t="n">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="G34" t="n">
-        <v>0.1614285714285714</v>
+        <v>0.1728571428571428</v>
       </c>
       <c r="H34" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I34" t="n">
-        <v>0.04666666666666667</v>
+        <v>0.04</v>
       </c>
       <c r="J34" t="n">
-        <v>0.1102362204724409</v>
+        <v>0.09022556390977443</v>
       </c>
       <c r="K34" t="n">
-        <v>1.241011200368038</v>
+        <v>1.463561035734032</v>
       </c>
       <c r="L34" t="n">
-        <v>0.1424208091850939</v>
+        <v>0.1944445376046642</v>
       </c>
       <c r="M34" t="n">
-        <v>1.300052983403203</v>
+        <v>1.313366602419445</v>
       </c>
       <c r="N34" t="n">
-        <v>0.3674540682414698</v>
+        <v>0.3007518796992481</v>
       </c>
       <c r="O34" t="n">
-        <v>7.394082671952995</v>
+        <v>7.555957015111813</v>
       </c>
     </row>
     <row r="35">
@@ -2719,40 +3974,40 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E35" t="n">
-        <v>0.097</v>
+        <v>0.093</v>
       </c>
       <c r="F35" t="n">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G35" t="n">
-        <v>0.1357142857142857</v>
+        <v>0.1285714285714286</v>
       </c>
       <c r="H35" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I35" t="n">
-        <v>0.006666666666666667</v>
+        <v>0.01</v>
       </c>
       <c r="J35" t="n">
-        <v>0.02061855670103093</v>
+        <v>0.03225806451612903</v>
       </c>
       <c r="K35" t="n">
-        <v>3.013281861902267</v>
+        <v>2.553799526274618</v>
       </c>
       <c r="L35" t="n">
-        <v>0.388856849797864</v>
+        <v>0.302807658115419</v>
       </c>
       <c r="M35" t="n">
-        <v>1.300052983403203</v>
+        <v>1.313366602419445</v>
       </c>
       <c r="N35" t="n">
-        <v>0.06872852233676977</v>
+        <v>0.1075268817204301</v>
       </c>
       <c r="O35" t="n">
-        <v>7.462811194289764</v>
+        <v>7.663483896832243</v>
       </c>
     </row>
     <row r="36">
@@ -2772,40 +4027,40 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E36" t="n">
-        <v>0.039</v>
+        <v>0.048</v>
       </c>
       <c r="F36" t="n">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="G36" t="n">
-        <v>0.05428571428571428</v>
+        <v>0.06571428571428571</v>
       </c>
       <c r="H36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I36" t="n">
-        <v>0.003333333333333334</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="J36" t="n">
-        <v>0.02564102564102564</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="K36" t="n">
-        <v>2.789988344330184</v>
+        <v>2.288046366790821</v>
       </c>
       <c r="L36" t="n">
-        <v>0.1421565489730141</v>
+        <v>0.1351036902295532</v>
       </c>
       <c r="M36" t="n">
-        <v>1.300052983403203</v>
+        <v>1.313366602419445</v>
       </c>
       <c r="N36" t="n">
-        <v>0.08547008547008547</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="O36" t="n">
-        <v>7.548281279759849</v>
+        <v>7.802372785721133</v>
       </c>
     </row>
     <row r="37">
@@ -2825,40 +4080,40 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E37" t="n">
-        <v>0.013</v>
+        <v>0.006</v>
       </c>
       <c r="F37" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G37" t="n">
-        <v>0.01571428571428572</v>
+        <v>0.008571428571428572</v>
       </c>
       <c r="H37" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I37" t="n">
-        <v>0.006666666666666667</v>
+        <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>0.1538461538461539</v>
+        <v>0</v>
       </c>
       <c r="K37" t="n">
-        <v>0.8573002431000968</v>
+        <v>9.056189692148925</v>
       </c>
       <c r="L37" t="n">
-        <v>0.007756526009000875</v>
+        <v>0.07762448307556222</v>
       </c>
       <c r="M37" t="n">
-        <v>1.300052983403203</v>
+        <v>1.313366602419445</v>
       </c>
       <c r="N37" t="n">
-        <v>0.5128205128205129</v>
+        <v>0</v>
       </c>
       <c r="O37" t="n">
-        <v>8.061101792580363</v>
+        <v>7.802372785721133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>